<commit_message>
Adding 'ENERGY_CARRIERS' to reference-case
Fixing a few typos in the database and adding it to the reference-case to fix workflows.
</commit_message>
<xml_diff>
--- a/cea/databases/CH/components/ENERGY_CARRIERS.xlsx
+++ b/cea/databases/CH/components/ENERGY_CARRIERS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiasniffeler/Documents/GitHub/CityEnergyAnalyst/cea/databases/SG/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276FF709-D20A-6A49-8940-20D036F3435C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5507ED2D-9D79-2047-BE7A-B8F420829D5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="2400" windowWidth="24680" windowHeight="16940" xr2:uid="{6334EB5C-C0D6-A34E-ABB5-EA8E490BB8B2}"/>
   </bookViews>
@@ -99,9 +99,6 @@
     <t>voltage</t>
   </si>
   <si>
-    <t>Sulight</t>
-  </si>
-  <si>
     <t>V</t>
   </si>
   <si>
@@ -142,9 +139,6 @@
   </si>
   <si>
     <t>Infrared light</t>
-  </si>
-  <si>
-    <t>ultraviolet</t>
   </si>
   <si>
     <t>chemical composition</t>
@@ -225,6 +219,12 @@
   </si>
   <si>
     <t>T60H</t>
+  </si>
+  <si>
+    <t>Sunlight</t>
+  </si>
+  <si>
+    <t>Ultraviolet</t>
   </si>
 </sst>
 </file>
@@ -702,7 +702,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -731,13 +731,13 @@
         <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>1</v>
@@ -771,7 +771,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>11</v>
@@ -849,7 +849,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="13">
         <v>230</v>
@@ -861,7 +861,7 @@
         <v>0.40570000000000001</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.2">
@@ -878,7 +878,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="11">
         <v>22000</v>
@@ -890,7 +890,7 @@
         <v>0.40570000000000001</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
@@ -907,7 +907,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="11">
         <v>66000</v>
@@ -919,21 +919,21 @@
         <v>0.40570000000000001</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -944,21 +944,21 @@
         <v>2.7E-2</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -969,21 +969,21 @@
         <v>2.8799999999999999E-2</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -994,21 +994,21 @@
         <v>2.8799999999999999E-2</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
@@ -1019,21 +1019,21 @@
         <v>0.41760000000000003</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="C13" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
@@ -1044,21 +1044,21 @@
         <v>0.3024</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="11"/>
@@ -1069,21 +1069,21 @@
         <v>0.24060000000000001</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="11"/>
@@ -1094,21 +1094,21 @@
         <v>0.12959999999999999</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="C16" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>34</v>
-      </c>
       <c r="D16" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="13"/>
@@ -1119,21 +1119,21 @@
         <v>1.9300000000000001E-2</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="D17" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="12"/>
@@ -1144,24 +1144,24 @@
         <v>0</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="D18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="F18" s="12">
         <v>200</v>
@@ -1169,24 +1169,24 @@
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="D19" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="F19" s="12">
         <v>1500</v>
@@ -1194,7 +1194,7 @@
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new optimisation to front-end
These changes introduce a new tab to the 'Optimization'-section of the front-end. Databases and the example reference case are also updated to match the new selection of components that can be installed in the supply system.
</commit_message>
<xml_diff>
--- a/cea/databases/CH/components/ENERGY_CARRIERS.xlsx
+++ b/cea/databases/CH/components/ENERGY_CARRIERS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiasniffeler/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EC0E18-F136-FD46-B76D-2B1DDD772316}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2AA1E5-DEC9-434C-B40F-A397EE551083}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{6334EB5C-C0D6-A34E-ABB5-EA8E490BB8B2}"/>
+    <workbookView xWindow="38400" yWindow="14860" windowWidth="25600" windowHeight="16000" xr2:uid="{6334EB5C-C0D6-A34E-ABB5-EA8E490BB8B2}"/>
   </bookViews>
   <sheets>
     <sheet name="ENERGY_CARRIERS" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="68">
   <si>
     <t>code</t>
   </si>
@@ -228,6 +228,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Warm water (room temperature)</t>
+  </si>
+  <si>
+    <t>T30H</t>
   </si>
 </sst>
 </file>
@@ -702,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DDCB6DC-A8A3-8E46-8CC9-FE356D9D4D97}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H19" sqref="E2:H19"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -802,10 +808,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>11</v>
@@ -816,8 +822,8 @@
       <c r="E4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="12">
-        <v>10</v>
+      <c r="F4" s="11">
+        <v>30</v>
       </c>
       <c r="G4" s="6">
         <v>0</v>
@@ -829,10 +835,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
@@ -843,8 +849,8 @@
       <c r="E5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="11">
-        <v>0</v>
+      <c r="F5" s="12">
+        <v>10</v>
       </c>
       <c r="G5" s="6">
         <v>0</v>
@@ -854,128 +860,126 @@
       </c>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" s="13">
-        <v>230</v>
-      </c>
-      <c r="G6" s="10">
-        <v>0.21</v>
-      </c>
-      <c r="H6" s="10">
-        <v>0.40570000000000001</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>49</v>
-      </c>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="11">
-        <v>22000</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0.18</v>
+      <c r="F7" s="13">
+        <v>230</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0.21</v>
       </c>
       <c r="H7" s="10">
         <v>0.40570000000000001</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="11">
-        <v>66000</v>
-      </c>
-      <c r="G8" s="6">
+        <v>22000</v>
+      </c>
+      <c r="G8" s="5">
         <v>0.18</v>
       </c>
       <c r="H8" s="10">
         <v>0.40570000000000001</v>
       </c>
       <c r="I8" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="11">
+        <v>66000</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0.18</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0.40570000000000001</v>
+      </c>
+      <c r="I9" s="9" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0.21</v>
-      </c>
-      <c r="H9" s="6">
-        <v>2.7E-2</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>33</v>
@@ -993,18 +997,18 @@
         <v>0.21</v>
       </c>
       <c r="H10" s="6">
-        <v>2.8799999999999999E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>33</v>
@@ -1030,10 +1034,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>33</v>
@@ -1051,18 +1055,18 @@
         <v>0.21</v>
       </c>
       <c r="H12" s="6">
-        <v>0.41760000000000003</v>
+        <v>2.8799999999999999E-2</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>33</v>
@@ -1077,21 +1081,21 @@
         <v>65</v>
       </c>
       <c r="G13" s="6">
-        <v>0.08</v>
+        <v>0.21</v>
       </c>
       <c r="H13" s="6">
-        <v>0.3024</v>
+        <v>0.41760000000000003</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>33</v>
@@ -1099,28 +1103,28 @@
       <c r="D14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" s="11" t="s">
+      <c r="E14" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>65</v>
       </c>
       <c r="G14" s="6">
-        <v>0.09</v>
-      </c>
-      <c r="H14" s="15">
-        <v>0.24060000000000001</v>
+        <v>0.08</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0.3024</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>33</v>
@@ -1135,76 +1139,76 @@
         <v>65</v>
       </c>
       <c r="G15" s="6">
-        <v>0.17</v>
-      </c>
-      <c r="H15" s="6">
-        <v>0.12959999999999999</v>
+        <v>0.09</v>
+      </c>
+      <c r="H15" s="15">
+        <v>0.24060000000000001</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="9" t="s">
+      <c r="A16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="G16" s="10">
+      <c r="E16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0.17</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0.12959999999999999</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="10">
         <v>0.2261</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H17" s="10">
         <v>1.9300000000000001E-2</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="I17" s="14" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G17" s="6">
-        <v>0</v>
-      </c>
-      <c r="H17" s="6">
-        <v>0</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>25</v>
@@ -1216,10 +1220,10 @@
         <v>34</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F18" s="12">
-        <v>200</v>
+        <v>65</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="G18" s="6">
         <v>0</v>
@@ -1233,7 +1237,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>25</v>
@@ -1248,15 +1252,44 @@
         <v>35</v>
       </c>
       <c r="F19" s="12">
+        <v>200</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="12">
         <v>1500</v>
       </c>
-      <c r="G19" s="6">
-        <v>0</v>
-      </c>
-      <c r="H19" s="6">
-        <v>0</v>
-      </c>
-      <c r="I19" s="9" t="s">
+      <c r="G20" s="6">
+        <v>0</v>
+      </c>
+      <c r="H20" s="6">
+        <v>0</v>
+      </c>
+      <c r="I20" s="9" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>